<commit_message>
Fixed BOM and 3D Printing Guide
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Beverage_Can_Opener_BOM.xlsx
+++ b/Documentation/Working_Documents/Beverage_Can_Opener_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tazo\Neil Squire\MMC-Everyone - Documents\Server\3 AT Library\WIP\Can Openers\Printlab_Beverage_Can_Opener\GitHub\Documentation\Working_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E96C7AE-530A-44EB-8C2A-9526F85CE177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5C9E29-4BE4-4CC1-AF9D-8DE9FD6E2399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>Beverage_Can_Opener.stl</t>
   </si>
   <si>
-    <t>https://github.com/makersmakingchange/Beverage_Can_Opener/settings</t>
+    <t>https://github.com/makersmakingchange/Beverage_Can_Opener/tree/main/Build_Files/3D_Print_Files</t>
   </si>
 </sst>
 </file>
@@ -693,7 +693,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,26 +831,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100456CAEA290209545A9F8681F83603874" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d27786a72e09a52c769a64d5f7eeaa24">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cf100d1-0775-4feb-8634-62999c4541bc" xmlns:ns3="38b325e6-602c-452a-8617-173bf47082c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03ae89856d271009074f70b56337b48d" ns2:_="" ns3:_="">
     <xsd:import namespace="8cf100d1-0775-4feb-8634-62999c4541bc"/>
@@ -1087,26 +1067,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99BECD52-63A8-454F-82E6-6195B786F95C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1123,4 +1104,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>